<commit_message>
Made progress on data flow
</commit_message>
<xml_diff>
--- a/doc/DataFlow.xlsx
+++ b/doc/DataFlow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
   <si>
     <t>HTML</t>
   </si>
@@ -397,6 +397,15 @@
   </si>
   <si>
     <t>own_URL3</t>
+  </si>
+  <si>
+    <t>finish_SA_click</t>
+  </si>
+  <si>
+    <t>aspects</t>
+  </si>
+  <si>
+    <t>aspects,traits,aspects_traits</t>
   </si>
 </sst>
 </file>
@@ -497,67 +506,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -905,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1438,14 +1387,25 @@
         <v>125</v>
       </c>
     </row>
+    <row r="39" spans="1:4" s="3" customFormat="1">
+      <c r="B39" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>"ISBLANK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added section for labeling self-aspects
</commit_message>
<xml_diff>
--- a/doc/DataFlow.xlsx
+++ b/doc/DataFlow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="143">
   <si>
     <t>HTML</t>
   </si>
@@ -406,13 +406,55 @@
   </si>
   <si>
     <t>aspects,traits,aspects_traits</t>
+  </si>
+  <si>
+    <t>self_aspects</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>aspectid</t>
+  </si>
+  <si>
+    <t>traitid</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>AspectId</t>
+  </si>
+  <si>
+    <t>TraitId</t>
+  </si>
+  <si>
+    <t>self_labeling_form</t>
+  </si>
+  <si>
+    <t>selfLabCheck</t>
+  </si>
+  <si>
+    <t>aspect_labs</t>
+  </si>
+  <si>
+    <t>(none)</t>
+  </si>
+  <si>
+    <t>self_labels</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -451,6 +493,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -481,7 +530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -489,24 +538,105 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -854,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1388,6 +1518,9 @@
       </c>
     </row>
     <row r="39" spans="1:4" s="3" customFormat="1">
+      <c r="A39" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="B39" s="3" t="s">
         <v>126</v>
       </c>
@@ -1398,14 +1531,98 @@
         <v>128</v>
       </c>
     </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="3" customFormat="1">
+      <c r="A43" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>"ISBLANK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="4">
+  <conditionalFormatting sqref="A1:D39 B40:D40 C41:D42 A40:A42 A43:D1048576">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added more data flow
</commit_message>
<xml_diff>
--- a/doc/DataFlow.xlsx
+++ b/doc/DataFlow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="17380" windowHeight="12420" tabRatio="500"/>
+    <workbookView xWindow="3860" yWindow="0" windowWidth="17380" windowHeight="12420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="153">
   <si>
     <t>HTML</t>
   </si>
@@ -448,6 +448,36 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>all_genself</t>
+  </si>
+  <si>
+    <t>checkGenSelf</t>
+  </si>
+  <si>
+    <t>selfqs</t>
+  </si>
+  <si>
+    <t>asp_gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">import </t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>checkSocMedia</t>
+  </si>
+  <si>
+    <t>facebookQs, twitterQs</t>
   </si>
 </sst>
 </file>
@@ -530,8 +560,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,7 +589,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -566,6 +598,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -574,9 +607,20 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -984,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1615,14 +1659,58 @@
         <v>142</v>
       </c>
     </row>
+    <row r="46" spans="1:4" s="3" customFormat="1">
+      <c r="A46" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="B48" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>"ISBLANK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D39 B40:D40 C41:D42 A40:A42 A43:D1048576">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="7" priority="4">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
more progress on DataFlow
</commit_message>
<xml_diff>
--- a/doc/DataFlow.xlsx
+++ b/doc/DataFlow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="0" windowWidth="17380" windowHeight="12420" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="60" windowWidth="17260" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="172">
   <si>
     <t>HTML</t>
   </si>
@@ -478,6 +478,63 @@
   </si>
   <si>
     <t>facebookQs, twitterQs</t>
+  </si>
+  <si>
+    <t>fb_feel</t>
+  </si>
+  <si>
+    <t>fb_feel_comments</t>
+  </si>
+  <si>
+    <t>fb_doing</t>
+  </si>
+  <si>
+    <t>fb_doing_comments</t>
+  </si>
+  <si>
+    <t>fb_where</t>
+  </si>
+  <si>
+    <t>fb_where_comments</t>
+  </si>
+  <si>
+    <t>fb_entertain</t>
+  </si>
+  <si>
+    <t>fb_entertain_comments</t>
+  </si>
+  <si>
+    <t>fb_political</t>
+  </si>
+  <si>
+    <t>fb_political_comments</t>
+  </si>
+  <si>
+    <t>fb_family</t>
+  </si>
+  <si>
+    <t>fb_family_comments</t>
+  </si>
+  <si>
+    <t>fb_god</t>
+  </si>
+  <si>
+    <t>fb_god_comments</t>
+  </si>
+  <si>
+    <t>fb_academic</t>
+  </si>
+  <si>
+    <t>fb_academic_comments</t>
+  </si>
+  <si>
+    <t>fb_appearance</t>
+  </si>
+  <si>
+    <t>fb_appearance_comments</t>
+  </si>
+  <si>
+    <t>aspects, survey</t>
   </si>
 </sst>
 </file>
@@ -560,8 +617,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -589,7 +648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -599,6 +658,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -608,79 +668,10 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1028,17 +1019,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
@@ -1695,22 +1686,115 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:4" s="3" customFormat="1">
+      <c r="A49" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>151</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="D50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="D51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="D52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="D53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="D54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="D55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="D56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="D57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="D58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="D59" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="D60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="D61" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="D62" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="D63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="D64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4">
+      <c r="D65" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4">
+      <c r="D66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4">
+      <c r="D67" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>"ISBLANK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D39 B40:D40 C41:D42 A40:A42 A43:D1048576">
-    <cfRule type="containsBlanks" dxfId="7" priority="4">
+  <conditionalFormatting sqref="A1:D39 B40:D40 C41:D42 A40:A42 A43:D49 A68:D1048576 A50:C67">
+    <cfRule type="containsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Some tweaks in data labels, work on self-aspects
</commit_message>
<xml_diff>
--- a/doc/DataFlow.xlsx
+++ b/doc/DataFlow.xlsx
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="172">
-  <si>
-    <t>HTML</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>PHP</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="173">
   <si>
     <t>&lt;form id="demographics"&gt;</t>
   </si>
@@ -165,48 +153,6 @@
     <t>party13</t>
   </si>
   <si>
-    <t>bond</t>
-  </si>
-  <si>
-    <t>solidarity</t>
-  </si>
-  <si>
-    <t>committed</t>
-  </si>
-  <si>
-    <t>glad</t>
-  </si>
-  <si>
-    <t>proud</t>
-  </si>
-  <si>
-    <t>pleasant</t>
-  </si>
-  <si>
-    <t>goodfeel</t>
-  </si>
-  <si>
-    <t>think</t>
-  </si>
-  <si>
-    <t>identity</t>
-  </si>
-  <si>
-    <t>seemyself</t>
-  </si>
-  <si>
-    <t>common_avg</t>
-  </si>
-  <si>
-    <t>similar_avg</t>
-  </si>
-  <si>
-    <t>common_oth</t>
-  </si>
-  <si>
-    <t>similar_oth</t>
-  </si>
-  <si>
     <t>qdata[0]</t>
   </si>
   <si>
@@ -300,102 +246,21 @@
     <t>freeform</t>
   </si>
   <si>
-    <t>free1</t>
-  </si>
-  <si>
-    <t>free2</t>
-  </si>
-  <si>
-    <t>user_url</t>
-  </si>
-  <si>
-    <t>free3</t>
-  </si>
-  <si>
-    <t>free4</t>
-  </si>
-  <si>
     <t>user_url2</t>
   </si>
   <si>
-    <t>free5</t>
-  </si>
-  <si>
-    <t>free6</t>
-  </si>
-  <si>
     <t>user_url3</t>
   </si>
   <si>
-    <t>nform1</t>
-  </si>
-  <si>
-    <t>nform2</t>
-  </si>
-  <si>
-    <t>userURL</t>
-  </si>
-  <si>
-    <t>nform3</t>
-  </si>
-  <si>
-    <t>nform4</t>
-  </si>
-  <si>
     <t>userURL2</t>
   </si>
   <si>
-    <t>nform5</t>
-  </si>
-  <si>
-    <t>nform6</t>
-  </si>
-  <si>
     <t>userURL3</t>
   </si>
   <si>
-    <t>ownform1</t>
-  </si>
-  <si>
-    <t>ownform2</t>
-  </si>
-  <si>
-    <t>ownform3</t>
-  </si>
-  <si>
-    <t>ownform4</t>
-  </si>
-  <si>
-    <t>ownform5</t>
-  </si>
-  <si>
-    <t>ownform6</t>
-  </si>
-  <si>
-    <t>own_form1</t>
-  </si>
-  <si>
-    <t>own_form2</t>
-  </si>
-  <si>
-    <t>own_URL</t>
-  </si>
-  <si>
-    <t>own_form3</t>
-  </si>
-  <si>
-    <t>own_form4</t>
-  </si>
-  <si>
     <t>own_URL2</t>
   </si>
   <si>
-    <t>own_form5</t>
-  </si>
-  <si>
-    <t>own_form6</t>
-  </si>
-  <si>
     <t>own_URL3</t>
   </si>
   <si>
@@ -535,6 +400,144 @@
   </si>
   <si>
     <t>aspects, survey</t>
+  </si>
+  <si>
+    <t>trial_newest.php</t>
+  </si>
+  <si>
+    <t>trial_newest.js</t>
+  </si>
+  <si>
+    <t>DataWrangler.php</t>
+  </si>
+  <si>
+    <t>identity.sql</t>
+  </si>
+  <si>
+    <t>party_com</t>
+  </si>
+  <si>
+    <t>own_form11</t>
+  </si>
+  <si>
+    <t>own_form12</t>
+  </si>
+  <si>
+    <t>own_URL1</t>
+  </si>
+  <si>
+    <t>own_form21</t>
+  </si>
+  <si>
+    <t>own_form22</t>
+  </si>
+  <si>
+    <t>own_form31</t>
+  </si>
+  <si>
+    <t>own_form32</t>
+  </si>
+  <si>
+    <t>ownform11</t>
+  </si>
+  <si>
+    <t>ownform12</t>
+  </si>
+  <si>
+    <t>userURL1</t>
+  </si>
+  <si>
+    <t>ownform21</t>
+  </si>
+  <si>
+    <t>ownform22</t>
+  </si>
+  <si>
+    <t>ownform31</t>
+  </si>
+  <si>
+    <t>ownform32</t>
+  </si>
+  <si>
+    <t>party0_bond</t>
+  </si>
+  <si>
+    <t>party1_solidarity</t>
+  </si>
+  <si>
+    <t>party2_committed</t>
+  </si>
+  <si>
+    <t>party3_glad</t>
+  </si>
+  <si>
+    <t>party4_proud</t>
+  </si>
+  <si>
+    <t>party5_pleasant</t>
+  </si>
+  <si>
+    <t>party6_goodfeel</t>
+  </si>
+  <si>
+    <t>party7_think</t>
+  </si>
+  <si>
+    <t>party8_identity</t>
+  </si>
+  <si>
+    <t>party9_seemyself</t>
+  </si>
+  <si>
+    <t>party10_common_avg</t>
+  </si>
+  <si>
+    <t>party11_similar_avg</t>
+  </si>
+  <si>
+    <t>party12_common_oth</t>
+  </si>
+  <si>
+    <t>party13_similar_oth</t>
+  </si>
+  <si>
+    <t>nform11</t>
+  </si>
+  <si>
+    <t>nform12</t>
+  </si>
+  <si>
+    <t>nform21</t>
+  </si>
+  <si>
+    <t>nform22</t>
+  </si>
+  <si>
+    <t>nform31</t>
+  </si>
+  <si>
+    <t>nform32</t>
+  </si>
+  <si>
+    <t>free11</t>
+  </si>
+  <si>
+    <t>free12</t>
+  </si>
+  <si>
+    <t>user_url1</t>
+  </si>
+  <si>
+    <t>free21</t>
+  </si>
+  <si>
+    <t>free22</t>
+  </si>
+  <si>
+    <t>free31</t>
+  </si>
+  <si>
+    <t>free32</t>
   </si>
 </sst>
 </file>
@@ -1019,772 +1022,779 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="560" topLeftCell="A17" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="3" customFormat="1">
-      <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="3" customFormat="1">
-      <c r="A29" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" t="s">
-        <v>117</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1">
+      <c r="A30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="D32" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="D34" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="D35" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="D37" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="3" customFormat="1">
-      <c r="A39" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B40" t="s">
-        <v>129</v>
-      </c>
-      <c r="C40" t="s">
-        <v>130</v>
-      </c>
-      <c r="D40" t="s">
-        <v>133</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="3" customFormat="1">
+      <c r="A40" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>129</v>
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>129</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="3" customFormat="1">
-      <c r="A43" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B44" t="s">
-        <v>140</v>
-      </c>
-      <c r="C44" t="s">
-        <v>130</v>
-      </c>
-      <c r="D44" t="s">
-        <v>133</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="3" customFormat="1">
+      <c r="A44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="3" customFormat="1">
-      <c r="A46" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="B47" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" t="s">
-        <v>147</v>
-      </c>
-      <c r="D47" t="s">
-        <v>148</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="B48" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1">
-      <c r="A49" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="D50" t="s">
-        <v>153</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1">
+      <c r="A50" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="D51" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="D52" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="D53" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="D54" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="D55" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="D56" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="D57" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="D58" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="D59" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="D60" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="D61" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="D62" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="D63" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="D64" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="4:4">
       <c r="D65" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="4:4">
       <c r="D66" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="4:4">
       <c r="D67" t="s">
-        <v>170</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4">
+      <c r="D68" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1793,7 +1803,7 @@
       <formula>"ISBLANK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D39 B40:D40 C41:D42 A40:A42 A43:D49 A68:D1048576 A50:C67">
+  <conditionalFormatting sqref="A1:D40 B41:D41 C42:D43 A41:A43 A44:D50 A69:D1048576 A51:C68">
     <cfRule type="containsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Finished all self-aspects components
</commit_message>
<xml_diff>
--- a/doc/DataFlow.xlsx
+++ b/doc/DataFlow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="238">
   <si>
     <t>&lt;form id="demographics"&gt;</t>
   </si>
@@ -538,6 +538,201 @@
   </si>
   <si>
     <t>free32</t>
+  </si>
+  <si>
+    <t>fb_express</t>
+  </si>
+  <si>
+    <t>sm_fbk</t>
+  </si>
+  <si>
+    <t>sm_gen[0]</t>
+  </si>
+  <si>
+    <t>sm_com[0]</t>
+  </si>
+  <si>
+    <t>sm_gen[1]</t>
+  </si>
+  <si>
+    <t>sm_com[1]</t>
+  </si>
+  <si>
+    <t>sm_gen[2]</t>
+  </si>
+  <si>
+    <t>sm_com[2]</t>
+  </si>
+  <si>
+    <t>sm_gen[3]</t>
+  </si>
+  <si>
+    <t>sm_com[3]</t>
+  </si>
+  <si>
+    <t>sm_gen[4]</t>
+  </si>
+  <si>
+    <t>sm_com[4]</t>
+  </si>
+  <si>
+    <t>sm_gen[5]</t>
+  </si>
+  <si>
+    <t>sm_com[5]</t>
+  </si>
+  <si>
+    <t>sm_gen[6]</t>
+  </si>
+  <si>
+    <t>sm_com[6]</t>
+  </si>
+  <si>
+    <t>sm_gen[7]</t>
+  </si>
+  <si>
+    <t>sm_com[7]</t>
+  </si>
+  <si>
+    <t>sm_gen[8]</t>
+  </si>
+  <si>
+    <t>sm_com[8]</t>
+  </si>
+  <si>
+    <t>smqs</t>
+  </si>
+  <si>
+    <t>fb_comments</t>
+  </si>
+  <si>
+    <t>sm_asp</t>
+  </si>
+  <si>
+    <t>smasps</t>
+  </si>
+  <si>
+    <t>smfbk</t>
+  </si>
+  <si>
+    <t>smqs[0]</t>
+  </si>
+  <si>
+    <t>smcomms[0]</t>
+  </si>
+  <si>
+    <t>smqs[1]</t>
+  </si>
+  <si>
+    <t>smqs[2]</t>
+  </si>
+  <si>
+    <t>smqs[3]</t>
+  </si>
+  <si>
+    <t>smqs[4]</t>
+  </si>
+  <si>
+    <t>smqs[5]</t>
+  </si>
+  <si>
+    <t>smqs[6]</t>
+  </si>
+  <si>
+    <t>smqs[7]</t>
+  </si>
+  <si>
+    <t>smqs[8]</t>
+  </si>
+  <si>
+    <t>smcomms[1]</t>
+  </si>
+  <si>
+    <t>smcomms[2]</t>
+  </si>
+  <si>
+    <t>smcomms[3]</t>
+  </si>
+  <si>
+    <t>smcomms[4]</t>
+  </si>
+  <si>
+    <t>smcomms[5]</t>
+  </si>
+  <si>
+    <t>smcomms[6]</t>
+  </si>
+  <si>
+    <t>smcomms[7]</t>
+  </si>
+  <si>
+    <t>smcomms[8]</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>tw_express</t>
+  </si>
+  <si>
+    <t>tw_comments</t>
+  </si>
+  <si>
+    <t>tw_feel</t>
+  </si>
+  <si>
+    <t>tw_feel_comments</t>
+  </si>
+  <si>
+    <t>tw_doing</t>
+  </si>
+  <si>
+    <t>tw_doing_comments</t>
+  </si>
+  <si>
+    <t>tw_where</t>
+  </si>
+  <si>
+    <t>tw_where_comments</t>
+  </si>
+  <si>
+    <t>tw_entertain</t>
+  </si>
+  <si>
+    <t>tw_entertain_comments</t>
+  </si>
+  <si>
+    <t>tw_political</t>
+  </si>
+  <si>
+    <t>tw_political_comments</t>
+  </si>
+  <si>
+    <t>tw_family</t>
+  </si>
+  <si>
+    <t>tw_family_comments</t>
+  </si>
+  <si>
+    <t>tw_god</t>
+  </si>
+  <si>
+    <t>tw_god_comments</t>
+  </si>
+  <si>
+    <t>tw_academic</t>
+  </si>
+  <si>
+    <t>tw_academic_comments</t>
+  </si>
+  <si>
+    <t>tw_appearance</t>
+  </si>
+  <si>
+    <t>tw_appearance_comments</t>
+  </si>
+  <si>
+    <t>Twitter</t>
   </si>
 </sst>
 </file>
@@ -620,8 +815,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -651,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -662,6 +867,11 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -672,9 +882,684 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1022,11 +1907,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="560" topLeftCell="A17" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="560" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1703,109 +2588,633 @@
       <c r="B50" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="C50" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="D50" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" t="s">
+        <v>197</v>
+      </c>
       <c r="D51" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="B52" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" t="s">
+        <v>198</v>
+      </c>
+      <c r="D52" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="D52" t="s">
+    <row r="53" spans="1:4">
+      <c r="B53" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" t="s">
+        <v>199</v>
+      </c>
+      <c r="D53" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="D53" t="s">
+    <row r="54" spans="1:4">
+      <c r="B54" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" t="s">
+        <v>200</v>
+      </c>
+      <c r="D54" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="D54" t="s">
+    <row r="55" spans="1:4">
+      <c r="B55" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" t="s">
+        <v>208</v>
+      </c>
+      <c r="D55" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="D55" t="s">
+    <row r="56" spans="1:4">
+      <c r="B56" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" t="s">
+        <v>201</v>
+      </c>
+      <c r="D56" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="D56" t="s">
+    <row r="57" spans="1:4">
+      <c r="B57" t="s">
+        <v>180</v>
+      </c>
+      <c r="C57" t="s">
+        <v>209</v>
+      </c>
+      <c r="D57" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="D57" t="s">
+    <row r="58" spans="1:4">
+      <c r="B58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" t="s">
+        <v>202</v>
+      </c>
+      <c r="D58" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="D58" t="s">
+    <row r="59" spans="1:4">
+      <c r="B59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C59" t="s">
+        <v>210</v>
+      </c>
+      <c r="D59" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="D59" t="s">
+    <row r="60" spans="1:4">
+      <c r="B60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" t="s">
+        <v>203</v>
+      </c>
+      <c r="D60" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="D60" t="s">
+    <row r="61" spans="1:4">
+      <c r="B61" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61" t="s">
+        <v>211</v>
+      </c>
+      <c r="D61" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="D61" t="s">
+    <row r="62" spans="1:4">
+      <c r="B62" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="D62" t="s">
+    <row r="63" spans="1:4">
+      <c r="B63" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" t="s">
+        <v>212</v>
+      </c>
+      <c r="D63" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="D63" t="s">
+    <row r="64" spans="1:4">
+      <c r="B64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" t="s">
+        <v>205</v>
+      </c>
+      <c r="D64" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="D64" t="s">
+    <row r="65" spans="1:4">
+      <c r="B65" t="s">
+        <v>188</v>
+      </c>
+      <c r="C65" t="s">
+        <v>213</v>
+      </c>
+      <c r="D65" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="4:4">
-      <c r="D65" t="s">
+    <row r="66" spans="1:4">
+      <c r="B66" t="s">
+        <v>189</v>
+      </c>
+      <c r="C66" t="s">
+        <v>206</v>
+      </c>
+      <c r="D66" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="4:4">
-      <c r="D66" t="s">
+    <row r="67" spans="1:4">
+      <c r="B67" t="s">
+        <v>190</v>
+      </c>
+      <c r="C67" t="s">
+        <v>214</v>
+      </c>
+      <c r="D67" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="4:4">
-      <c r="D67" t="s">
+    <row r="68" spans="1:4">
+      <c r="B68" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="68" spans="4:4">
-      <c r="D68" t="s">
+    <row r="69" spans="1:4">
+      <c r="B69" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" t="s">
+        <v>215</v>
+      </c>
+      <c r="D69" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="B70" t="s">
+        <v>195</v>
+      </c>
+      <c r="C70" t="s">
+        <v>196</v>
+      </c>
+      <c r="D70" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>217</v>
+      </c>
+      <c r="B71" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" t="s">
+        <v>197</v>
+      </c>
+      <c r="D71" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="B72" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="B73" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" t="s">
+        <v>199</v>
+      </c>
+      <c r="D73" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="B74" t="s">
+        <v>177</v>
+      </c>
+      <c r="C74" t="s">
+        <v>200</v>
+      </c>
+      <c r="D74" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="B75" t="s">
+        <v>178</v>
+      </c>
+      <c r="C75" t="s">
+        <v>208</v>
+      </c>
+      <c r="D75" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="B76" t="s">
+        <v>179</v>
+      </c>
+      <c r="C76" t="s">
+        <v>201</v>
+      </c>
+      <c r="D76" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="B77" t="s">
+        <v>180</v>
+      </c>
+      <c r="C77" t="s">
+        <v>209</v>
+      </c>
+      <c r="D77" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="B78" t="s">
+        <v>181</v>
+      </c>
+      <c r="C78" t="s">
+        <v>202</v>
+      </c>
+      <c r="D78" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="B79" t="s">
+        <v>182</v>
+      </c>
+      <c r="C79" t="s">
+        <v>210</v>
+      </c>
+      <c r="D79" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="B80" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" t="s">
+        <v>203</v>
+      </c>
+      <c r="D80" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" t="s">
+        <v>211</v>
+      </c>
+      <c r="D81" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" t="s">
+        <v>185</v>
+      </c>
+      <c r="C82" t="s">
+        <v>204</v>
+      </c>
+      <c r="D82" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" t="s">
+        <v>186</v>
+      </c>
+      <c r="C83" t="s">
+        <v>212</v>
+      </c>
+      <c r="D83" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" t="s">
+        <v>187</v>
+      </c>
+      <c r="C84" t="s">
+        <v>205</v>
+      </c>
+      <c r="D84" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" t="s">
+        <v>188</v>
+      </c>
+      <c r="C85" t="s">
+        <v>213</v>
+      </c>
+      <c r="D85" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86" t="s">
+        <v>206</v>
+      </c>
+      <c r="D86" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" t="s">
+        <v>190</v>
+      </c>
+      <c r="C87" t="s">
+        <v>214</v>
+      </c>
+      <c r="D87" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88" t="s">
+        <v>207</v>
+      </c>
+      <c r="D88" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" t="s">
+        <v>192</v>
+      </c>
+      <c r="C89" t="s">
+        <v>215</v>
+      </c>
+      <c r="D89" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" t="s">
+        <v>195</v>
+      </c>
+      <c r="C90" t="s">
+        <v>196</v>
+      </c>
+      <c r="D90" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="68" priority="35">
       <formula>"ISBLANK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D40 B41:D41 C42:D43 A41:A43 A44:D50 A69:D1048576 A51:C68">
-    <cfRule type="containsBlanks" dxfId="0" priority="4">
+  <conditionalFormatting sqref="A1:D40 B41:D41 C42:D43 A41:A43 B70:D70 B52:C53 A44:D47 A91:D1048576 A71 A50:D51 B48:D49">
+    <cfRule type="containsBlanks" dxfId="67" priority="37">
       <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54:B55">
+    <cfRule type="containsBlanks" dxfId="66" priority="33">
+      <formula>LEN(TRIM(B54))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56:B57">
+    <cfRule type="containsBlanks" dxfId="64" priority="32">
+      <formula>LEN(TRIM(B56))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58:B59">
+    <cfRule type="containsBlanks" dxfId="62" priority="31">
+      <formula>LEN(TRIM(B58))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60:B61">
+    <cfRule type="containsBlanks" dxfId="60" priority="30">
+      <formula>LEN(TRIM(B60))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62:B63">
+    <cfRule type="containsBlanks" dxfId="58" priority="29">
+      <formula>LEN(TRIM(B62))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64:B65">
+    <cfRule type="containsBlanks" dxfId="56" priority="28">
+      <formula>LEN(TRIM(B64))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66:B67">
+    <cfRule type="containsBlanks" dxfId="54" priority="27">
+      <formula>LEN(TRIM(B66))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68:B69">
+    <cfRule type="containsBlanks" dxfId="52" priority="26">
+      <formula>LEN(TRIM(B68))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsBlanks" dxfId="49" priority="25">
+      <formula>LEN(TRIM(C54))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="containsBlanks" dxfId="47" priority="24">
+      <formula>LEN(TRIM(C56))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58:C59">
+    <cfRule type="containsBlanks" dxfId="45" priority="23">
+      <formula>LEN(TRIM(C58))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C61">
+    <cfRule type="containsBlanks" dxfId="43" priority="22">
+      <formula>LEN(TRIM(C60))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62:C63">
+    <cfRule type="containsBlanks" dxfId="41" priority="21">
+      <formula>LEN(TRIM(C62))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64:C65">
+    <cfRule type="containsBlanks" dxfId="39" priority="20">
+      <formula>LEN(TRIM(C64))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66:C67">
+    <cfRule type="containsBlanks" dxfId="37" priority="19">
+      <formula>LEN(TRIM(C66))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C69">
+    <cfRule type="containsBlanks" dxfId="35" priority="18">
+      <formula>LEN(TRIM(C68))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B90:D90 B72:C73 B71:D71">
+    <cfRule type="containsBlanks" dxfId="33" priority="17">
+      <formula>LEN(TRIM(B71))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74:B75">
+    <cfRule type="containsBlanks" dxfId="31" priority="16">
+      <formula>LEN(TRIM(B74))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B76:B77">
+    <cfRule type="containsBlanks" dxfId="29" priority="15">
+      <formula>LEN(TRIM(B76))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B78:B79">
+    <cfRule type="containsBlanks" dxfId="27" priority="14">
+      <formula>LEN(TRIM(B78))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80:B81">
+    <cfRule type="containsBlanks" dxfId="25" priority="13">
+      <formula>LEN(TRIM(B80))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82:B83">
+    <cfRule type="containsBlanks" dxfId="23" priority="12">
+      <formula>LEN(TRIM(B82))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84:B85">
+    <cfRule type="containsBlanks" dxfId="21" priority="11">
+      <formula>LEN(TRIM(B84))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B86:B87">
+    <cfRule type="containsBlanks" dxfId="19" priority="10">
+      <formula>LEN(TRIM(B86))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B88:B89">
+    <cfRule type="containsBlanks" dxfId="17" priority="9">
+      <formula>LEN(TRIM(B88))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74:C75">
+    <cfRule type="containsBlanks" dxfId="15" priority="8">
+      <formula>LEN(TRIM(C74))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76:C77">
+    <cfRule type="containsBlanks" dxfId="13" priority="7">
+      <formula>LEN(TRIM(C76))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C78:C79">
+    <cfRule type="containsBlanks" dxfId="11" priority="6">
+      <formula>LEN(TRIM(C78))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C80:C81">
+    <cfRule type="containsBlanks" dxfId="9" priority="5">
+      <formula>LEN(TRIM(C80))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C83">
+    <cfRule type="containsBlanks" dxfId="7" priority="4">
+      <formula>LEN(TRIM(C82))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84:C85">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
+      <formula>LEN(TRIM(C84))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C86:C87">
+    <cfRule type="containsBlanks" dxfId="3" priority="2">
+      <formula>LEN(TRIM(C86))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88:C89">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(C88))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed small bugs for final implementation
</commit_message>
<xml_diff>
--- a/doc/DataFlow.xlsx
+++ b/doc/DataFlow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="239">
   <si>
     <t>&lt;form id="demographics"&gt;</t>
   </si>
@@ -733,6 +733,9 @@
   </si>
   <si>
     <t>Twitter</t>
+  </si>
+  <si>
+    <t>pol_spec</t>
   </si>
 </sst>
 </file>
@@ -815,8 +818,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -856,7 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -872,6 +877,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -887,329 +893,10 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1911,7 +1598,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2091,11 +1778,29 @@
       <c r="A13" t="s">
         <v>131</v>
       </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>23</v>
       </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D14" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
@@ -3043,167 +2748,167 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="68" priority="35">
+    <cfRule type="expression" dxfId="36" priority="35">
       <formula>"ISBLANK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D40 B41:D41 C42:D43 A41:A43 B70:D70 B52:C53 A44:D47 A91:D1048576 A71 A50:D51 B48:D49">
-    <cfRule type="containsBlanks" dxfId="67" priority="37">
+  <conditionalFormatting sqref="B41:D41 C42:D43 A41:A43 B70:D70 B52:C53 A44:D47 A91:D1048576 A71 A50:D51 B48:D49 A1:D40">
+    <cfRule type="containsBlanks" dxfId="35" priority="37">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:B55">
-    <cfRule type="containsBlanks" dxfId="66" priority="33">
+    <cfRule type="containsBlanks" dxfId="34" priority="33">
       <formula>LEN(TRIM(B54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56:B57">
-    <cfRule type="containsBlanks" dxfId="64" priority="32">
+    <cfRule type="containsBlanks" dxfId="33" priority="32">
       <formula>LEN(TRIM(B56))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58:B59">
-    <cfRule type="containsBlanks" dxfId="62" priority="31">
+    <cfRule type="containsBlanks" dxfId="32" priority="31">
       <formula>LEN(TRIM(B58))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60:B61">
-    <cfRule type="containsBlanks" dxfId="60" priority="30">
+    <cfRule type="containsBlanks" dxfId="31" priority="30">
       <formula>LEN(TRIM(B60))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:B63">
-    <cfRule type="containsBlanks" dxfId="58" priority="29">
+    <cfRule type="containsBlanks" dxfId="30" priority="29">
       <formula>LEN(TRIM(B62))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64:B65">
-    <cfRule type="containsBlanks" dxfId="56" priority="28">
+    <cfRule type="containsBlanks" dxfId="29" priority="28">
       <formula>LEN(TRIM(B64))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66:B67">
-    <cfRule type="containsBlanks" dxfId="54" priority="27">
+    <cfRule type="containsBlanks" dxfId="28" priority="27">
       <formula>LEN(TRIM(B66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68:B69">
-    <cfRule type="containsBlanks" dxfId="52" priority="26">
+    <cfRule type="containsBlanks" dxfId="27" priority="26">
       <formula>LEN(TRIM(B68))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsBlanks" dxfId="49" priority="25">
+    <cfRule type="containsBlanks" dxfId="26" priority="25">
       <formula>LEN(TRIM(C54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="containsBlanks" dxfId="47" priority="24">
+    <cfRule type="containsBlanks" dxfId="25" priority="24">
       <formula>LEN(TRIM(C56))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C59">
-    <cfRule type="containsBlanks" dxfId="45" priority="23">
+    <cfRule type="containsBlanks" dxfId="24" priority="23">
       <formula>LEN(TRIM(C58))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C61">
-    <cfRule type="containsBlanks" dxfId="43" priority="22">
+    <cfRule type="containsBlanks" dxfId="23" priority="22">
       <formula>LEN(TRIM(C60))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62:C63">
-    <cfRule type="containsBlanks" dxfId="41" priority="21">
+    <cfRule type="containsBlanks" dxfId="22" priority="21">
       <formula>LEN(TRIM(C62))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:C65">
-    <cfRule type="containsBlanks" dxfId="39" priority="20">
+    <cfRule type="containsBlanks" dxfId="21" priority="20">
       <formula>LEN(TRIM(C64))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C67">
-    <cfRule type="containsBlanks" dxfId="37" priority="19">
+    <cfRule type="containsBlanks" dxfId="20" priority="19">
       <formula>LEN(TRIM(C66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C69">
-    <cfRule type="containsBlanks" dxfId="35" priority="18">
+    <cfRule type="containsBlanks" dxfId="19" priority="18">
       <formula>LEN(TRIM(C68))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90:D90 B72:C73 B71:D71">
-    <cfRule type="containsBlanks" dxfId="33" priority="17">
+    <cfRule type="containsBlanks" dxfId="18" priority="17">
       <formula>LEN(TRIM(B71))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74:B75">
-    <cfRule type="containsBlanks" dxfId="31" priority="16">
+    <cfRule type="containsBlanks" dxfId="17" priority="16">
       <formula>LEN(TRIM(B74))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B77">
-    <cfRule type="containsBlanks" dxfId="29" priority="15">
+    <cfRule type="containsBlanks" dxfId="16" priority="15">
       <formula>LEN(TRIM(B76))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78:B79">
-    <cfRule type="containsBlanks" dxfId="27" priority="14">
+    <cfRule type="containsBlanks" dxfId="15" priority="14">
       <formula>LEN(TRIM(B78))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81">
-    <cfRule type="containsBlanks" dxfId="25" priority="13">
+    <cfRule type="containsBlanks" dxfId="14" priority="13">
       <formula>LEN(TRIM(B80))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B83">
-    <cfRule type="containsBlanks" dxfId="23" priority="12">
+    <cfRule type="containsBlanks" dxfId="13" priority="12">
       <formula>LEN(TRIM(B82))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84:B85">
-    <cfRule type="containsBlanks" dxfId="21" priority="11">
+    <cfRule type="containsBlanks" dxfId="12" priority="11">
       <formula>LEN(TRIM(B84))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86:B87">
-    <cfRule type="containsBlanks" dxfId="19" priority="10">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(B86))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B89">
-    <cfRule type="containsBlanks" dxfId="17" priority="9">
+    <cfRule type="containsBlanks" dxfId="10" priority="9">
       <formula>LEN(TRIM(B88))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74:C75">
-    <cfRule type="containsBlanks" dxfId="15" priority="8">
+    <cfRule type="containsBlanks" dxfId="9" priority="8">
       <formula>LEN(TRIM(C74))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76:C77">
-    <cfRule type="containsBlanks" dxfId="13" priority="7">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(C76))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78:C79">
-    <cfRule type="containsBlanks" dxfId="11" priority="6">
+    <cfRule type="containsBlanks" dxfId="7" priority="6">
       <formula>LEN(TRIM(C78))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80:C81">
-    <cfRule type="containsBlanks" dxfId="9" priority="5">
+    <cfRule type="containsBlanks" dxfId="6" priority="5">
       <formula>LEN(TRIM(C80))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C83">
-    <cfRule type="containsBlanks" dxfId="7" priority="4">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(C82))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84:C85">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+    <cfRule type="containsBlanks" dxfId="4" priority="3">
       <formula>LEN(TRIM(C84))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3213,7 +2918,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C88))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>